<commit_message>
Updated data description and download guide with population, NDVI, and Elevation data instructions
</commit_message>
<xml_diff>
--- a/data_description.xlsx
+++ b/data_description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\profu\Documents\Schoolwork\Postdoc\Research Projects\no2_modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\profu\Documents\Schoolwork\Postdoc\Research Projects\no2_model_mexico_city\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5FBB39-6534-4D66-93EE-3A21341D272C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98213A68-9CDA-4085-A443-8C4AC6A2149A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{482C9871-EA23-4559-A058-2642FF904522}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="106">
   <si>
     <t>name</t>
   </si>
@@ -362,9 +362,6 @@
     <t>MOD13Q1 v006</t>
   </si>
   <si>
-    <t>ndvi</t>
-  </si>
-  <si>
     <t>250m</t>
   </si>
   <si>
@@ -380,9 +377,6 @@
     <t>pop_density</t>
   </si>
   <si>
-    <t>evi</t>
-  </si>
-  <si>
     <t>Gridded Population of the World (GPW), v4</t>
   </si>
   <si>
@@ -402,6 +396,42 @@
   </si>
   <si>
     <t>Roads, etc.</t>
+  </si>
+  <si>
+    <t>elevation</t>
+  </si>
+  <si>
+    <t>NASA Shuttle Radar Topography Mission (SRTMGL1)</t>
+  </si>
+  <si>
+    <t>1 arc second</t>
+  </si>
+  <si>
+    <t>once</t>
+  </si>
+  <si>
+    <t>elevation data</t>
+  </si>
+  <si>
+    <t>ndvi_250m</t>
+  </si>
+  <si>
+    <t>evi_250m</t>
+  </si>
+  <si>
+    <t>ndvi_1km</t>
+  </si>
+  <si>
+    <t>MOD13A3 v006</t>
+  </si>
+  <si>
+    <t>30-day</t>
+  </si>
+  <si>
+    <t>1km</t>
+  </si>
+  <si>
+    <t>slightly lower resolution NDVI product; sufficient for purposes of NO2 model</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1256,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27A4CA7-AF7A-4701-8352-E97DC3482A45}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1656,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
         <v>81</v>
@@ -1638,18 +1668,18 @@
         <v>20191231</v>
       </c>
       <c r="E18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
         <v>84</v>
-      </c>
-      <c r="F18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
         <v>81</v>
@@ -1661,41 +1691,41 @@
         <v>20191231</v>
       </c>
       <c r="E19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C20">
-        <v>2000</v>
+        <v>20050101</v>
       </c>
       <c r="D20">
-        <v>2020</v>
+        <v>20191231</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="G20" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" t="s">
         <v>87</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
       </c>
       <c r="C21">
         <v>2000</v>
@@ -1704,24 +1734,67 @@
         <v>2020</v>
       </c>
       <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" t="s">
         <v>90</v>
-      </c>
-      <c r="F21" t="s">
-        <v>91</v>
-      </c>
-      <c r="G21" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22">
+        <v>2000</v>
+      </c>
+      <c r="D22">
+        <v>2020</v>
+      </c>
+      <c r="E22" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" t="s">
+        <v>89</v>
+      </c>
+      <c r="G22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" t="s">
         <v>93</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>94</v>
       </c>
-      <c r="G22" t="s">
+      <c r="B24" t="s">
         <v>95</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>